<commit_message>
adding email logic and email form logic and appending data into database
</commit_message>
<xml_diff>
--- a/Backend/public/uploads/Book1.xlsx
+++ b/Backend/public/uploads/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vaibh\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6BDF35-9715-42ED-8495-ED0ECA229D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E56001-AE05-46B9-AF36-0FB46B11DAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4215" yWindow="2430" windowWidth="21600" windowHeight="11295" xr2:uid="{6ED153B4-890B-4744-94E5-9F812CFBB1BA}"/>
   </bookViews>
@@ -33,10 +33,10 @@
     <t>vaibhavv</t>
   </si>
   <si>
-    <t>vaibhavzade8021@gmail.com</t>
+    <t>vaibhavzade802@gmail.com</t>
   </si>
   <si>
-    <t>vaibhavzade1591@gmail.com</t>
+    <t>vaibhavzade159@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>